<commit_message>
Backend Done for now
</commit_message>
<xml_diff>
--- a/Database Separations.xlsx
+++ b/Database Separations.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bhira\Documents\GitHub\MiniProject-Celebrities\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75481ADD-742B-4D9A-BC57-1409F0A1ACDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA6F9F38-5594-4F5C-BBB1-14007B18A0FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{3214CEC4-2312-4B59-B6CF-E63D5012AC0A}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="40">
   <si>
     <t>Celebrities</t>
   </si>
@@ -616,6 +616,27 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
@@ -662,27 +683,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1000,8 +1000,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CDAB30FB-B2E3-4C05-8831-8A75E7F62BAE}">
   <dimension ref="A1:J17"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L6" sqref="L6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1244,7 +1244,7 @@
   <dimension ref="A1:D36"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A28" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+      <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1257,37 +1257,37 @@
       <c r="A1" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="39" t="s">
+      <c r="B1" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="C1" s="40"/>
+      <c r="C1" s="19"/>
     </row>
     <row r="2" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="34">
+      <c r="A2" s="20">
         <v>1</v>
       </c>
-      <c r="B2" s="37" t="s">
+      <c r="B2" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="38"/>
+      <c r="C2" s="24"/>
     </row>
     <row r="3" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="35"/>
-      <c r="B3" s="37" t="s">
+      <c r="A3" s="21"/>
+      <c r="B3" s="23" t="s">
         <v>25</v>
       </c>
-      <c r="C3" s="38"/>
+      <c r="C3" s="24"/>
     </row>
     <row r="4" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="35"/>
-      <c r="B4" s="37" t="s">
+      <c r="A4" s="21"/>
+      <c r="B4" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="38"/>
+      <c r="C4" s="24"/>
     </row>
     <row r="5" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="35"/>
-      <c r="B5" s="34" t="s">
+      <c r="A5" s="21"/>
+      <c r="B5" s="20" t="s">
         <v>8</v>
       </c>
       <c r="C5" s="6" t="s">
@@ -1295,45 +1295,45 @@
       </c>
     </row>
     <row r="6" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="35"/>
-      <c r="B6" s="35"/>
+      <c r="A6" s="21"/>
+      <c r="B6" s="21"/>
       <c r="C6" s="6" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="36"/>
-      <c r="B7" s="36"/>
+      <c r="A7" s="22"/>
+      <c r="B7" s="22"/>
       <c r="C7" s="6" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="34">
+      <c r="A8" s="20">
         <v>2</v>
       </c>
-      <c r="B8" s="37" t="s">
+      <c r="B8" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="38"/>
+      <c r="C8" s="24"/>
     </row>
     <row r="9" spans="1:3" ht="28.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="35"/>
-      <c r="B9" s="37" t="s">
+      <c r="A9" s="21"/>
+      <c r="B9" s="23" t="s">
         <v>26</v>
       </c>
-      <c r="C9" s="38"/>
+      <c r="C9" s="24"/>
     </row>
     <row r="10" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="35"/>
-      <c r="B10" s="37" t="s">
+      <c r="A10" s="21"/>
+      <c r="B10" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="C10" s="38"/>
+      <c r="C10" s="24"/>
     </row>
     <row r="11" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="35"/>
-      <c r="B11" s="34" t="s">
+      <c r="A11" s="21"/>
+      <c r="B11" s="20" t="s">
         <v>8</v>
       </c>
       <c r="C11" s="6" t="s">
@@ -1341,45 +1341,45 @@
       </c>
     </row>
     <row r="12" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="35"/>
-      <c r="B12" s="35"/>
+      <c r="A12" s="21"/>
+      <c r="B12" s="21"/>
       <c r="C12" s="6" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="36"/>
-      <c r="B13" s="36"/>
+      <c r="A13" s="22"/>
+      <c r="B13" s="22"/>
       <c r="C13" s="6" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="34">
+      <c r="A14" s="20">
         <v>3</v>
       </c>
-      <c r="B14" s="37" t="s">
+      <c r="B14" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="C14" s="38"/>
+      <c r="C14" s="24"/>
     </row>
     <row r="15" spans="1:3" ht="28.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="35"/>
-      <c r="B15" s="37" t="s">
+      <c r="A15" s="21"/>
+      <c r="B15" s="23" t="s">
         <v>27</v>
       </c>
-      <c r="C15" s="38"/>
+      <c r="C15" s="24"/>
     </row>
     <row r="16" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="35"/>
-      <c r="B16" s="37" t="s">
+      <c r="A16" s="21"/>
+      <c r="B16" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="C16" s="38"/>
+      <c r="C16" s="24"/>
     </row>
     <row r="17" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="35"/>
-      <c r="B17" s="34" t="s">
+      <c r="A17" s="21"/>
+      <c r="B17" s="20" t="s">
         <v>8</v>
       </c>
       <c r="C17" s="6" t="s">
@@ -1387,15 +1387,15 @@
       </c>
     </row>
     <row r="18" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="35"/>
-      <c r="B18" s="35"/>
+      <c r="A18" s="21"/>
+      <c r="B18" s="21"/>
       <c r="C18" s="6" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="36"/>
-      <c r="B19" s="36"/>
+      <c r="A19" s="22"/>
+      <c r="B19" s="22"/>
       <c r="C19" s="6" t="s">
         <v>22</v>
       </c>
@@ -1406,11 +1406,11 @@
       <c r="C20" s="7"/>
     </row>
     <row r="21" spans="1:4" ht="28.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="20" t="s">
+      <c r="A21" s="27" t="s">
         <v>28</v>
       </c>
-      <c r="B21" s="21"/>
-      <c r="C21" s="22"/>
+      <c r="B21" s="28"/>
+      <c r="C21" s="29"/>
     </row>
     <row r="22" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" s="7"/>
@@ -1423,11 +1423,11 @@
       <c r="C23" s="7"/>
     </row>
     <row r="24" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="23" t="s">
+      <c r="A24" s="30" t="s">
         <v>29</v>
       </c>
-      <c r="B24" s="24"/>
-      <c r="C24" s="25"/>
+      <c r="B24" s="31"/>
+      <c r="C24" s="32"/>
     </row>
     <row r="25" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25" s="8"/>
@@ -1438,10 +1438,10 @@
       <c r="A26" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="B26" s="26" t="s">
+      <c r="B26" s="33" t="s">
         <v>30</v>
       </c>
-      <c r="C26" s="27"/>
+      <c r="C26" s="34"/>
       <c r="D26" s="11" t="s">
         <v>38</v>
       </c>
@@ -1450,10 +1450,10 @@
       <c r="A27" s="10">
         <v>1</v>
       </c>
-      <c r="B27" s="28" t="s">
+      <c r="B27" s="35" t="s">
         <v>31</v>
       </c>
-      <c r="C27" s="29"/>
+      <c r="C27" s="36"/>
       <c r="D27" s="13" t="s">
         <v>39</v>
       </c>
@@ -1462,10 +1462,10 @@
       <c r="A28" s="5">
         <v>2</v>
       </c>
-      <c r="B28" s="30" t="s">
+      <c r="B28" s="37" t="s">
         <v>32</v>
       </c>
-      <c r="C28" s="31"/>
+      <c r="C28" s="38"/>
       <c r="D28" s="14" t="s">
         <v>39</v>
       </c>
@@ -1474,40 +1474,46 @@
       <c r="A29" s="12">
         <v>3</v>
       </c>
-      <c r="B29" s="32" t="s">
+      <c r="B29" s="39" t="s">
         <v>33</v>
       </c>
-      <c r="C29" s="33"/>
-      <c r="D29" s="15"/>
+      <c r="C29" s="40"/>
+      <c r="D29" s="15" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="30" spans="1:4" ht="57.6" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A30" s="10">
         <v>4</v>
       </c>
-      <c r="B30" s="18" t="s">
+      <c r="B30" s="25" t="s">
         <v>34</v>
       </c>
-      <c r="C30" s="19"/>
-      <c r="D30" s="15"/>
+      <c r="C30" s="26"/>
+      <c r="D30" s="15" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="31" spans="1:4" ht="43.2" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A31" s="10">
         <v>5</v>
       </c>
-      <c r="B31" s="18" t="s">
+      <c r="B31" s="25" t="s">
         <v>35</v>
       </c>
-      <c r="C31" s="19"/>
-      <c r="D31" s="15"/>
+      <c r="C31" s="26"/>
+      <c r="D31" s="15" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="32" spans="1:4" ht="28.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A32" s="10">
         <v>6</v>
       </c>
-      <c r="B32" s="18" t="s">
+      <c r="B32" s="25" t="s">
         <v>36</v>
       </c>
-      <c r="C32" s="19"/>
+      <c r="C32" s="26"/>
       <c r="D32" s="16" t="s">
         <v>39</v>
       </c>
@@ -1516,10 +1522,10 @@
       <c r="A33" s="10">
         <v>7</v>
       </c>
-      <c r="B33" s="18" t="s">
+      <c r="B33" s="25" t="s">
         <v>37</v>
       </c>
-      <c r="C33" s="19"/>
+      <c r="C33" s="26"/>
       <c r="D33" s="15" t="s">
         <v>39</v>
       </c>
@@ -1535,22 +1541,6 @@
     </row>
   </sheetData>
   <mergeCells count="26">
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="A2:A7"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B5:B7"/>
-    <mergeCell ref="A14:A19"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="B17:B19"/>
-    <mergeCell ref="A8:A13"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B11:B13"/>
     <mergeCell ref="B30:C30"/>
     <mergeCell ref="B31:C31"/>
     <mergeCell ref="B32:C32"/>
@@ -1561,6 +1551,22 @@
     <mergeCell ref="B27:C27"/>
     <mergeCell ref="B28:C28"/>
     <mergeCell ref="B29:C29"/>
+    <mergeCell ref="A8:A13"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B11:B13"/>
+    <mergeCell ref="A14:A19"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B17:B19"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="A2:A7"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B5:B7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>